<commit_message>
updated plan version for code release
</commit_message>
<xml_diff>
--- a/PMP/ReleasePlanning_fourthRelease_FoodiesWebApp_v1.xlsx
+++ b/PMP/ReleasePlanning_fourthRelease_FoodiesWebApp_v1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sagedwael/QA project/release 4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sagedwael/Documents/GitHub/QA-Workshop_Foodies/PMP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F2E5E6E-1677-904E-8A1F-BE8CDB20515B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F317E302-3393-2C44-AA68-7A52E3A574AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="17340" xr2:uid="{E9C65AA8-DBCD-8542-AAC2-582E5FCA2851}"/>
   </bookViews>
@@ -62,21 +62,9 @@
     <t>saged</t>
   </si>
   <si>
-    <t>UI-Login</t>
-  </si>
-  <si>
     <t>mariam ahmed</t>
   </si>
   <si>
-    <t>UI-HomeScreen</t>
-  </si>
-  <si>
-    <t>UI-Restaurant Page</t>
-  </si>
-  <si>
-    <t>UI-Offers</t>
-  </si>
-  <si>
     <t>atef</t>
   </si>
   <si>
@@ -86,9 +74,6 @@
     <t>Youssef</t>
   </si>
   <si>
-    <t>UI-Checkout</t>
-  </si>
-  <si>
     <t>FodiesWebApp_Release003_WPK002</t>
   </si>
   <si>
@@ -117,9 +102,6 @@
   </si>
   <si>
     <t>PM TASKS</t>
-  </si>
-  <si>
-    <t>PMP_comments&amp;fix</t>
   </si>
   <si>
     <t>TRELLO_task creation and assignment</t>
@@ -202,13 +184,31 @@
   </si>
   <si>
     <t>mariam moustafa</t>
+  </si>
+  <si>
+    <t>PMP_comments&amp;fix(Review)</t>
+  </si>
+  <si>
+    <t>UI-Login+design issues</t>
+  </si>
+  <si>
+    <t>UI-HomeScreen+design issues</t>
+  </si>
+  <si>
+    <t>UI-Restaurant Page+design issues</t>
+  </si>
+  <si>
+    <t>UI-Offers+design issues</t>
+  </si>
+  <si>
+    <t>UI-Checkout+design issues</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -236,8 +236,13 @@
       <color theme="1"/>
       <name val="Apple Braille"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Aptos Narrow (Body)"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -292,6 +297,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -305,7 +316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -363,6 +374,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -700,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6775EA5B-4169-EA4A-9AB0-726D1B01DC2C}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="110" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -736,13 +753,13 @@
         <v>5</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>
@@ -754,10 +771,10 @@
       <c r="A3" s="21"/>
       <c r="B3" s="21"/>
       <c r="C3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>
@@ -769,10 +786,10 @@
       <c r="A4" s="21"/>
       <c r="B4" s="21"/>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E4" s="2">
         <v>1</v>
@@ -784,10 +801,10 @@
       <c r="A5" s="21"/>
       <c r="B5" s="21"/>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E5" s="2">
         <v>1</v>
@@ -799,10 +816,10 @@
       <c r="A6" s="21"/>
       <c r="B6" s="21"/>
       <c r="C6" s="2" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E6" s="2">
         <v>1</v>
@@ -814,10 +831,10 @@
       <c r="A7" s="21"/>
       <c r="B7" s="21"/>
       <c r="C7" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E7" s="2">
         <v>1</v>
@@ -829,10 +846,10 @@
       <c r="A8" s="21"/>
       <c r="B8" s="21"/>
       <c r="C8" s="2" t="s">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E8" s="2">
         <v>1</v>
@@ -851,16 +868,16 @@
     </row>
     <row r="10" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="22" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E10" s="3">
         <v>6</v>
@@ -872,10 +889,10 @@
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E11" s="3">
         <v>6</v>
@@ -887,10 +904,10 @@
       <c r="A12" s="22"/>
       <c r="B12" s="23"/>
       <c r="C12" s="3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E12" s="3">
         <v>3</v>
@@ -902,10 +919,10 @@
       <c r="A13" s="22"/>
       <c r="B13" s="23"/>
       <c r="C13" s="3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E13" s="3">
         <v>6</v>
@@ -917,10 +934,10 @@
       <c r="A14" s="22"/>
       <c r="B14" s="23"/>
       <c r="C14" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E14" s="3">
         <v>3</v>
@@ -932,10 +949,10 @@
       <c r="A15" s="22"/>
       <c r="B15" s="23"/>
       <c r="C15" s="3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E15" s="3">
         <v>3</v>
@@ -947,10 +964,10 @@
       <c r="A16" s="22"/>
       <c r="B16" s="23"/>
       <c r="C16" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E16" s="3">
         <v>3</v>
@@ -961,14 +978,14 @@
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="17"/>
       <c r="B17" s="18"/>
-      <c r="C17" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="3">
-        <v>3</v>
+      <c r="C17" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="24">
+        <v>0</v>
       </c>
       <c r="F17" s="12"/>
       <c r="G17" s="12"/>
@@ -976,27 +993,27 @@
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="17"/>
       <c r="B18" s="18"/>
-      <c r="C18" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" s="3">
-        <v>10</v>
+      <c r="C18" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="24">
+        <v>0</v>
       </c>
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="19" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>7</v>
@@ -1011,7 +1028,7 @@
       <c r="A20" s="19"/>
       <c r="B20" s="19"/>
       <c r="C20" s="4" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>7</v>
@@ -1026,7 +1043,7 @@
       <c r="A21" s="19"/>
       <c r="B21" s="19"/>
       <c r="C21" s="4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>7</v>
@@ -1039,16 +1056,16 @@
     </row>
     <row r="22" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="20" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E22" s="4">
         <v>3</v>
@@ -1060,10 +1077,10 @@
       <c r="A23" s="20"/>
       <c r="B23" s="20"/>
       <c r="C23" s="9" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E23" s="4">
         <v>3</v>
@@ -1075,10 +1092,10 @@
       <c r="A24" s="20"/>
       <c r="B24" s="20"/>
       <c r="C24" s="9" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="E24" s="4">
         <v>3</v>
@@ -1090,10 +1107,10 @@
       <c r="A25" s="20"/>
       <c r="B25" s="20"/>
       <c r="C25" s="9" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="E25" s="4">
         <v>3</v>
@@ -1105,10 +1122,10 @@
       <c r="A26" s="20"/>
       <c r="B26" s="20"/>
       <c r="C26" s="9" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="E26" s="4">
         <v>3</v>
@@ -1120,10 +1137,10 @@
       <c r="A27" s="20"/>
       <c r="B27" s="20"/>
       <c r="C27" s="9" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E27" s="4">
         <v>3</v>
@@ -1135,10 +1152,10 @@
       <c r="A28" s="20"/>
       <c r="B28" s="20"/>
       <c r="C28" s="9" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E28" s="4">
         <v>2</v>
@@ -1150,10 +1167,10 @@
       <c r="A29" s="20"/>
       <c r="B29" s="20"/>
       <c r="C29" s="9" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E29" s="13">
         <v>3</v>
@@ -1163,139 +1180,139 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="F31" s="14"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B32" s="5">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C32" s="5">
-        <f>SUM(E18,E21,E19,E20)</f>
-        <v>19</v>
+        <f>SUM(E19,E20,E21,E22,E23,E25,E24,E26,E27,E28,E29)</f>
+        <v>32</v>
       </c>
       <c r="D32" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="15"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B33" s="5">
         <v>12</v>
       </c>
       <c r="C33" s="5">
-        <f>SUM(E14,E12,E29,E27)</f>
-        <v>12</v>
+        <f>SUM(E4,E6,E12,E14)</f>
+        <v>8</v>
       </c>
       <c r="D33" s="5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E33" s="5"/>
       <c r="F33" s="15"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B34" s="5">
         <v>12</v>
       </c>
       <c r="C34" s="5">
-        <f>SUM(E7,E8,E15,E16,E25)</f>
-        <v>11</v>
+        <f>SUM(E7,E8,E15,E16)</f>
+        <v>8</v>
       </c>
       <c r="D34" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="15"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B35" s="5">
         <v>12</v>
       </c>
       <c r="C35" s="5">
-        <f>SUM(E3,E11,E22,E28)</f>
-        <v>12</v>
+        <f>SUM(E3,E11)</f>
+        <v>7</v>
       </c>
       <c r="D35" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="15"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B36" s="5">
         <v>12</v>
       </c>
       <c r="C36" s="5">
-        <f>SUM(E2,E10,E23)</f>
-        <v>10</v>
+        <f>SUM(E2,E10)</f>
+        <v>7</v>
       </c>
       <c r="D36" s="5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="15"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B37" s="5">
         <v>13</v>
       </c>
       <c r="C37" s="5">
-        <f>SUM(E5,E13,E24,E26)</f>
-        <v>13</v>
+        <f>SUM(E13,E5)</f>
+        <v>7</v>
       </c>
       <c r="D37" s="5">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E37" s="5"/>
       <c r="F37" s="15"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B38" s="5">
         <f>SUM(B32:B37)</f>
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="C38" s="5">
         <f>SUM(C32:C37)</f>
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D38" s="5">
         <f>SUM(D32:D37)</f>
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="E38" s="5">
         <f>SUM(E32:E37)</f>

</xml_diff>

<commit_message>
update this is the third version
</commit_message>
<xml_diff>
--- a/PMP/ReleasePlanning_fourthRelease_FoodiesWebApp_v1.xlsx
+++ b/PMP/ReleasePlanning_fourthRelease_FoodiesWebApp_v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sagedwael/Documents/GitHub/QA-Workshop_Foodies/PMP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F317E302-3393-2C44-AA68-7A52E3A574AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F21A8E-AB90-C64A-88C0-114FC0EC03A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="17340" xr2:uid="{E9C65AA8-DBCD-8542-AAC2-582E5FCA2851}"/>
   </bookViews>
@@ -718,7 +718,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>